<commit_message>
Inclusão da tela de Vistoria
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -1042,7 +1042,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1185,7 +1185,7 @@
       <c r="I4" s="4"/>
       <c r="K4" s="27">
         <f>AVERAGE(G8:G24)</f>
-        <v>0.41470588235294115</v>
+        <v>0.44117647058823528</v>
       </c>
       <c r="L4" s="28"/>
       <c r="M4" s="28"/>
@@ -1663,7 +1663,7 @@
         <v>10</v>
       </c>
       <c r="F14" s="15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G14" s="16">
         <v>1</v>
@@ -1680,13 +1680,13 @@
         <v>5</v>
       </c>
       <c r="E15" s="15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F15" s="15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G15" s="16">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>